<commit_message>
Missed a header when updating an Environment table.
</commit_message>
<xml_diff>
--- a/docs/Figures/EnvironmentWorking.xlsx
+++ b/docs/Figures/EnvironmentWorking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-135" windowWidth="23700" windowHeight="11955"/>
+    <workbookView xWindow="-60" yWindow="-135" windowWidth="23700" windowHeight="11955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EnvironmentVariables" sheetId="17" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="216">
   <si>
     <t>Description</t>
   </si>
@@ -1273,9 +1273,6 @@
   </si>
   <si>
     <t xml:space="preserve">ISO 7730:2005 </t>
-  </si>
-  <si>
-    <t>BioGears</t>
   </si>
   <si>
     <t>Inputs</t>
@@ -4116,7 +4113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:I63"/>
     </sheetView>
   </sheetViews>
@@ -4176,7 +4173,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4194,10 +4191,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4215,10 +4212,10 @@
         <v>21</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4236,10 +4233,10 @@
         <v>25</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -4257,10 +4254,10 @@
         <v>29</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4276,10 +4273,10 @@
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4295,10 +4292,10 @@
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4314,10 +4311,10 @@
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -4336,7 +4333,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4352,10 +4349,10 @@
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4371,10 +4368,10 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4388,10 +4385,10 @@
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4405,10 +4402,10 @@
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4422,10 +4419,10 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4439,10 +4436,10 @@
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4456,10 +4453,10 @@
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4473,10 +4470,10 @@
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
@@ -4492,10 +4489,10 @@
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4511,10 +4508,10 @@
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4530,10 +4527,10 @@
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -4549,10 +4546,10 @@
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -4568,10 +4565,10 @@
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4587,10 +4584,10 @@
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -4606,10 +4603,10 @@
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -4628,7 +4625,7 @@
         <v>81</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4644,10 +4641,10 @@
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4663,10 +4660,10 @@
       </c>
       <c r="F29" s="23"/>
       <c r="G29" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4682,10 +4679,10 @@
       </c>
       <c r="F30" s="23"/>
       <c r="G30" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -4701,10 +4698,10 @@
       </c>
       <c r="F31" s="23"/>
       <c r="G31" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -4720,10 +4717,10 @@
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4739,10 +4736,10 @@
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4758,10 +4755,10 @@
       </c>
       <c r="F34" s="23"/>
       <c r="G34" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -4777,10 +4774,10 @@
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -4796,10 +4793,10 @@
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="18" x14ac:dyDescent="0.25">
@@ -6146,8 +6143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:V34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:V18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6162,7 +6159,7 @@
     <row r="1" spans="5:22" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="5:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
@@ -6170,7 +6167,7 @@
       <c r="I2" s="69"/>
       <c r="J2" s="70"/>
       <c r="K2" s="68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L2" s="69"/>
       <c r="M2" s="69"/>
@@ -6182,51 +6179,51 @@
       <c r="S2" s="69"/>
       <c r="T2" s="71"/>
       <c r="U2" s="68" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="V2" s="70"/>
     </row>
     <row r="3" spans="5:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="G3" s="75" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="H3" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="I3" s="75" t="s">
         <v>184</v>
       </c>
-      <c r="I3" s="75" t="s">
+      <c r="J3" s="78" t="s">
         <v>185</v>
       </c>
-      <c r="J3" s="78" t="s">
+      <c r="K3" s="85" t="s">
         <v>186</v>
-      </c>
-      <c r="K3" s="85" t="s">
-        <v>187</v>
       </c>
       <c r="L3" s="87"/>
       <c r="M3" s="81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N3" s="82"/>
       <c r="O3" s="85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P3" s="87"/>
       <c r="Q3" s="81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R3" s="82"/>
       <c r="S3" s="85" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T3" s="86"/>
       <c r="U3" s="72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V3" s="78"/>
     </row>
@@ -6261,37 +6258,37 @@
         <v>176</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M5" s="54" t="s">
         <v>176</v>
       </c>
       <c r="N5" s="58" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O5" s="46" t="s">
         <v>176</v>
       </c>
       <c r="P5" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q5" s="54" t="s">
         <v>176</v>
       </c>
       <c r="R5" s="58" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S5" s="46" t="s">
         <v>176</v>
       </c>
       <c r="T5" s="58" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="U5" s="46" t="s">
         <v>176</v>
       </c>
       <c r="V5" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="5:22" x14ac:dyDescent="0.25">

</xml_diff>